<commit_message>
Form got a threaded rod to move
</commit_message>
<xml_diff>
--- a/Bom.xlsx
+++ b/Bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC7E05BF-B093-4EC2-AE7C-80829CD18D88}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E70728D-7DDC-4B30-A94E-63A825EC1072}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1946,13 +1946,13 @@
     <t>https://www.kugellager-express.de/miniatur-kugellager-mr74-zz-4x7x2-5-mm</t>
   </si>
   <si>
-    <t>https://www.ebay.de/itm/Linearer-Kugellager-langer-Serie-1pcs-LM6LUU-6-mm-Motion-Liner-Ball-bushing/232391646779?ssPageName=STRK%3AMEBIDX%3AIT&amp;_trksid=p2060353.m2749.l2649</t>
-  </si>
-  <si>
-    <t>Form linear bearing</t>
-  </si>
-  <si>
-    <t>linear bearing LM6 lUU, 6x12x35mm</t>
+    <t>https://www.pololu.com/product/3432</t>
+  </si>
+  <si>
+    <t>Rotational Servo Parallax 360°</t>
+  </si>
+  <si>
+    <t>Form Lifting Servo</t>
   </si>
 </sst>
 </file>
@@ -5472,10 +5472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M19"/>
+  <dimension ref="B2:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5979,7 +5979,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="394">
-        <f t="shared" ref="I17:I18" si="4">INT((B17-1-L17)/H17+1)</f>
+        <f t="shared" ref="I17" si="4">INT((B17-1-L17)/H17+1)</f>
         <v>4</v>
       </c>
       <c r="J17" s="395">
@@ -5995,13 +5995,13 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="394">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="394" t="s">
+        <v>641</v>
+      </c>
+      <c r="D18" s="394" t="s">
         <v>642</v>
-      </c>
-      <c r="D18" s="394" t="s">
-        <v>641</v>
       </c>
       <c r="G18" s="391" t="s">
         <v>640</v>
@@ -6010,24 +6010,33 @@
         <v>1</v>
       </c>
       <c r="I18" s="394">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J18" s="395">
-        <v>1.5</v>
+        <v>29.9</v>
       </c>
       <c r="K18" s="392">
         <f t="shared" si="5"/>
-        <v>4.5</v>
+        <v>29.9</v>
       </c>
       <c r="L18" s="394">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="K19" s="393">
-        <f>SUM(K3:K11)</f>
-        <v>119.94999999999999</v>
+      <c r="B19" s="394"/>
+      <c r="C19" s="394"/>
+      <c r="D19" s="394"/>
+      <c r="H19" s="394"/>
+      <c r="I19" s="394"/>
+      <c r="J19" s="395"/>
+      <c r="K19" s="392"/>
+      <c r="L19" s="394"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="K20" s="393">
+        <f>SUM(K3:K17)</f>
+        <v>192.82999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>